<commit_message>
Add domain & deity generators & routers
</commit_message>
<xml_diff>
--- a/city-npc/Ptolus_City_NPC_Encounter.xlsx
+++ b/city-npc/Ptolus_City_NPC_Encounter.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="START" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="433">
   <si>
     <t xml:space="preserve">MORTAL</t>
   </si>
@@ -1094,7 +1094,7 @@
     <t xml:space="preserve">Zealot</t>
   </si>
   <si>
-    <t xml:space="preserve">CLERIC DOMAINS</t>
+    <t xml:space="preserve">Divine Domains (Generator)</t>
   </si>
   <si>
     <t xml:space="preserve">CIVILIZATION</t>
@@ -1109,7 +1109,16 @@
     <t xml:space="preserve">Life</t>
   </si>
   <si>
-    <t xml:space="preserve">Cleric Domains</t>
+    <t xml:space="preserve">Key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arcana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arcana</t>
   </si>
   <si>
     <t xml:space="preserve">Civilization</t>
@@ -1121,7 +1130,7 @@
     <t xml:space="preserve">Knowledge</t>
   </si>
   <si>
-    <t xml:space="preserve">Arcana</t>
+    <t xml:space="preserve">civilization</t>
   </si>
   <si>
     <t xml:space="preserve">Asche, God of Cities</t>
@@ -1130,6 +1139,9 @@
     <t xml:space="preserve">Heiran, Sister of Death</t>
   </si>
   <si>
+    <t xml:space="preserve">death</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nareis, Sister of Death</t>
   </si>
   <si>
@@ -1139,6 +1151,12 @@
     <t xml:space="preserve">Gaen, Goddess of Light</t>
   </si>
   <si>
+    <t xml:space="preserve">grave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grave</t>
+  </si>
+  <si>
     <t xml:space="preserve">Unnah, Mistress of the Blades</t>
   </si>
   <si>
@@ -1148,46 +1166,76 @@
     <t xml:space="preserve">Melann, Goddess of Farming</t>
   </si>
   <si>
-    <t xml:space="preserve">Grave</t>
+    <t xml:space="preserve">knowledge</t>
   </si>
   <si>
     <t xml:space="preserve">Locharit, the Goddess of the Written Word</t>
   </si>
   <si>
+    <t xml:space="preserve">life</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mocharum, God of Dwarves</t>
   </si>
   <si>
     <t xml:space="preserve">Tevra, the Clockwork Goddess</t>
   </si>
   <si>
+    <t xml:space="preserve">light</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Light</t>
+  </si>
+  <si>
     <t xml:space="preserve">Teun, Mother of All Machines</t>
   </si>
   <si>
-    <t xml:space="preserve">Light</t>
+    <t xml:space="preserve">luck</t>
   </si>
   <si>
     <t xml:space="preserve">Luck</t>
   </si>
   <si>
+    <t xml:space="preserve">nature</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nature</t>
   </si>
   <si>
+    <t xml:space="preserve">night</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Night</t>
+  </si>
+  <si>
     <t xml:space="preserve">Protection</t>
   </si>
   <si>
-    <t xml:space="preserve">Night</t>
+    <t xml:space="preserve">order</t>
   </si>
   <si>
     <t xml:space="preserve">Order</t>
   </si>
   <si>
+    <t xml:space="preserve">peace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">protection</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Lady</t>
   </si>
   <si>
     <t xml:space="preserve">Ahaar, Lord of the Air</t>
   </si>
   <si>
-    <t xml:space="preserve">Peace</t>
+    <t xml:space="preserve">technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technology</t>
   </si>
   <si>
     <t xml:space="preserve">Rajek the Wanderer</t>
@@ -1196,34 +1244,85 @@
     <t xml:space="preserve">Harredda, Mistress of Ravens</t>
   </si>
   <si>
+    <t xml:space="preserve">tempest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tempest</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Fifty-Three Gods of Chance</t>
   </si>
   <si>
     <t xml:space="preserve">Navashtrom, God of Strength and Harmony</t>
   </si>
   <si>
-    <t xml:space="preserve">Technology</t>
+    <t xml:space="preserve">travel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travel</t>
   </si>
   <si>
     <t xml:space="preserve">Myliesha, Mistress of the Wind’s Path</t>
   </si>
   <si>
-    <t xml:space="preserve">Tempest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Travel</t>
+    <t xml:space="preserve">trickery</t>
   </si>
   <si>
     <t xml:space="preserve">Trickery</t>
   </si>
   <si>
+    <t xml:space="preserve">twilight</t>
+  </si>
+  <si>
     <t xml:space="preserve">Twilight</t>
   </si>
   <si>
+    <t xml:space="preserve">war</t>
+  </si>
+  <si>
     <t xml:space="preserve">War</t>
   </si>
   <si>
+    <t xml:space="preserve">Deity (Router)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placeholder</t>
+  </si>
+  <si>
     <t xml:space="preserve">Inurath, Mistress of War</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[generator:deity-28death29-soullink|{}|deity]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[generator:deity-28knowledge29-soullink|{}|deity]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[generator:deity-28life29-soullink|{}|deity]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[generator:deity-28light29-soullink|{}|deity]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[generator:deity-28luck29-soullink|{}|deity]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[generator:deity-28nature29-soullink|{}|deity]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[generator:deity-28protection29-soullink|{}|deity]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[generator:deity-28technology29-soullink|{}|deity]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[generator:deity-28tempest29-soullink|{}|deity]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[generator:deity-28trickery29-soullink|{}|deity]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[generator:deity-28war29-soullink|{}|deity]</t>
   </si>
 </sst>
 </file>
@@ -3809,8 +3908,8 @@
   </sheetPr>
   <dimension ref="A2:AMJ118"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H37" activeCellId="0" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5482,19 +5581,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:O29"/>
+  <dimension ref="B2:R45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="1.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="1.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="1.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.6"/>
@@ -5505,40 +5604,51 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="25.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="1.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="25.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="8.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="1.61"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="E2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="0"/>
       <c r="F2" s="3"/>
       <c r="G2" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="3"/>
       <c r="J2" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="3"/>
       <c r="M2" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="3"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="P2" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <f aca="false">SUM(D4:D22)</f>
+        <v>162</v>
+      </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -5550,617 +5660,862 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <f aca="false">SUM(B5:B23)</f>
-        <v>160</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>362</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <f aca="false">SUM(E5:E10)</f>
-        <v>100</v>
-      </c>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>364</v>
+      </c>
+      <c r="D4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0"/>
       <c r="G4" s="7" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="H4" s="5" t="n">
         <f aca="false">SUM(H5:H10)</f>
         <v>100</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="K4" s="5" t="n">
         <f aca="false">SUM(K5:K10)</f>
         <v>100</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="N4" s="5" t="n">
         <f aca="false">SUM(N5:N10)</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
+      <c r="P4" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q4" s="5" t="n">
+        <f aca="false">SUM(Q5:Q10)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>365</v>
       </c>
-      <c r="B5" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E5" s="0"/>
+      <c r="G5" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="N5" s="10" t="n">
+        <v>30</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="Q5" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>366</v>
       </c>
-      <c r="E5" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="G5" s="0" t="s">
+      <c r="D6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" s="0"/>
+      <c r="J6" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>373</v>
+      </c>
+      <c r="N6" s="10" t="n">
+        <v>10</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="Q6" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0"/>
+      <c r="J7" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="N7" s="10" t="n">
+        <v>20</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q7" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>367</v>
       </c>
-      <c r="H5" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>366</v>
-      </c>
-      <c r="K5" s="10" t="n">
-        <v>30</v>
-      </c>
-      <c r="M5" s="0" t="s">
-        <v>366</v>
-      </c>
-      <c r="N5" s="1" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>362</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>368</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>369</v>
-      </c>
-      <c r="K6" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="M6" s="0" t="s">
-        <v>370</v>
-      </c>
-      <c r="N6" s="1" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>363</v>
-      </c>
-      <c r="B7" s="1" t="n">
+      <c r="D8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>371</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>372</v>
-      </c>
-      <c r="K7" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>373</v>
-      </c>
-      <c r="N7" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>374</v>
-      </c>
-      <c r="B8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="5"/>
+      <c r="E8" s="0"/>
       <c r="G8" s="7"/>
       <c r="H8" s="5"/>
-      <c r="J8" s="12" t="s">
-        <v>375</v>
-      </c>
-      <c r="K8" s="10" t="n">
+      <c r="J8" s="7"/>
+      <c r="K8" s="5"/>
+      <c r="M8" s="12" t="s">
+        <v>381</v>
+      </c>
+      <c r="N8" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="M8" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="N8" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>364</v>
-      </c>
-      <c r="B9" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="5"/>
+      <c r="P8" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q8" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E9" s="0"/>
       <c r="G9" s="7"/>
       <c r="H9" s="5"/>
-      <c r="J9" s="12" t="s">
-        <v>376</v>
-      </c>
-      <c r="K9" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="M9" s="0" t="s">
-        <v>377</v>
-      </c>
-      <c r="N9" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>360</v>
-      </c>
-      <c r="B10" s="1" t="n">
+      <c r="J9" s="7"/>
+      <c r="K9" s="5"/>
+      <c r="M9" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="N9" s="10" t="n">
+        <v>10</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="Q9" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="D10" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="5"/>
+      <c r="E10" s="0"/>
       <c r="G10" s="7"/>
       <c r="H10" s="5"/>
-      <c r="J10" s="0" t="s">
-        <v>378</v>
-      </c>
-      <c r="K10" s="10" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>379</v>
-      </c>
-      <c r="B11" s="1" t="n">
+      <c r="J10" s="7"/>
+      <c r="K10" s="5"/>
+      <c r="M10" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="N10" s="10" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="D11" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="5"/>
+      <c r="E11" s="0"/>
       <c r="G11" s="7"/>
       <c r="H11" s="5"/>
-      <c r="J11" s="12"/>
+      <c r="J11" s="7"/>
       <c r="K11" s="5"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="s">
+      <c r="M11" s="12"/>
+      <c r="N11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E12" s="0"/>
+      <c r="H12" s="0"/>
+      <c r="K12" s="0"/>
+      <c r="N12" s="0"/>
+      <c r="Q12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="0"/>
+      <c r="G13" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="N13" s="2"/>
+      <c r="P13" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="0"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="0"/>
+      <c r="G15" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <f aca="false">SUM(H16:H21)</f>
+        <v>100</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K15" s="5" t="n">
+        <f aca="false">SUM(K16:K21)</f>
+        <v>100</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="N15" s="5" t="n">
+        <f aca="false">SUM(N16:N21)</f>
+        <v>100</v>
+      </c>
+      <c r="P15" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q15" s="5" t="n">
+        <f aca="false">SUM(Q16:Q21)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E16" s="0"/>
+      <c r="G16" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="H16" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="M16" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="N16" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="P16" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q16" s="1" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E17" s="0"/>
+      <c r="G17" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="M17" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="N17" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="P17" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="Q17" s="1" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E18" s="0"/>
+      <c r="G18" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="K18" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="N18" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="P18" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="Q18" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="0"/>
+      <c r="G19" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>412</v>
+      </c>
+      <c r="N19" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="P19" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="Q19" s="1" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E20" s="0"/>
+      <c r="G20" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="H20" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="P20" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="Q20" s="1" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>416</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="0"/>
+      <c r="G21" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D23" s="0"/>
+      <c r="H23" s="0"/>
+      <c r="K23" s="0"/>
+      <c r="N23" s="0"/>
+      <c r="Q23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="H24" s="2"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="K24" s="2"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="N24" s="2"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="Q24" s="2"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="G26" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="H26" s="5" t="n">
+        <f aca="false">SUM(H27:H32)</f>
+        <v>100</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="K26" s="5" t="n">
+        <f aca="false">SUM(K27:K32)</f>
+        <v>100</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="N26" s="5" t="n">
+        <f aca="false">SUM(N27:N32)</f>
+        <v>100</v>
+      </c>
+      <c r="P26" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="Q26" s="5" t="n">
+        <f aca="false">SUM(Q27:Q32)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="D27" s="10"/>
+      <c r="G27" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="H27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="K27" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="M27" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="N27" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="P27" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q27" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="H28" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="K28" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="M28" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="N28" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="P28" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="Q28" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="H29" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="K29" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="M29" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="N29" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="P29" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q29" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>412</v>
+      </c>
+      <c r="K30" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="s">
         <v>380</v>
       </c>
-      <c r="B12" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="K12" s="2"/>
-      <c r="M12" s="2" t="s">
+      <c r="C31" s="0" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
         <v>382</v>
       </c>
-      <c r="N12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>381</v>
-      </c>
-      <c r="B13" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>383</v>
-      </c>
-      <c r="B14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>379</v>
-      </c>
-      <c r="E14" s="5" t="n">
-        <f aca="false">SUM(E15:E20)</f>
-        <v>100</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>380</v>
-      </c>
-      <c r="H14" s="5" t="n">
-        <f aca="false">SUM(H15:H20)</f>
-        <v>100</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>381</v>
-      </c>
-      <c r="K14" s="5" t="n">
-        <f aca="false">SUM(K15:K20)</f>
-        <v>100</v>
-      </c>
-      <c r="M14" s="7" t="s">
-        <v>382</v>
-      </c>
-      <c r="N14" s="5" t="n">
-        <f aca="false">SUM(N15:N20)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>384</v>
-      </c>
-      <c r="B15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>370</v>
-      </c>
-      <c r="E15" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="G15" s="0" t="s">
+      <c r="C32" s="0" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="s">
         <v>385</v>
       </c>
-      <c r="H15" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>386</v>
-      </c>
-      <c r="K15" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="M15" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="N15" s="1" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>387</v>
-      </c>
-      <c r="B16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>372</v>
-      </c>
-      <c r="E16" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="G16" s="0" t="s">
+      <c r="C33" s="0" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="12" t="s">
         <v>388</v>
       </c>
-      <c r="H16" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>389</v>
-      </c>
-      <c r="K16" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="M16" s="0" t="s">
-        <v>389</v>
-      </c>
-      <c r="N16" s="1" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>382</v>
-      </c>
-      <c r="B17" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>375</v>
-      </c>
-      <c r="E17" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="G17" s="0" t="s">
+      <c r="C34" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="D34" s="10"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
         <v>390</v>
       </c>
-      <c r="H17" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>373</v>
-      </c>
-      <c r="K17" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="M17" s="0" t="s">
-        <v>391</v>
-      </c>
-      <c r="N17" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="C35" s="0" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
         <v>392</v>
       </c>
-      <c r="B18" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>373</v>
-      </c>
-      <c r="E18" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>393</v>
-      </c>
-      <c r="K18" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="M18" s="0" t="s">
-        <v>388</v>
-      </c>
-      <c r="N18" s="1" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>394</v>
-      </c>
-      <c r="B19" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>391</v>
-      </c>
-      <c r="E19" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="M19" s="0" t="s">
-        <v>385</v>
-      </c>
-      <c r="N19" s="1" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="C36" s="0" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
         <v>395</v>
       </c>
-      <c r="B20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>378</v>
-      </c>
-      <c r="E20" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>396</v>
-      </c>
-      <c r="B21" s="1" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="C37" s="0" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="B22" s="1" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="B23" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="K23" s="2"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="N23" s="2"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="7" t="s">
-        <v>392</v>
-      </c>
-      <c r="E25" s="5" t="n">
-        <f aca="false">SUM(E26:E31)</f>
-        <v>100</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>394</v>
-      </c>
-      <c r="H25" s="5" t="n">
-        <f aca="false">SUM(H26:H31)</f>
-        <v>100</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>396</v>
-      </c>
-      <c r="K25" s="5" t="n">
-        <f aca="false">SUM(K26:K31)</f>
-        <v>100</v>
-      </c>
-      <c r="M25" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="N25" s="5" t="n">
-        <f aca="false">SUM(N26:N31)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="0" t="s">
-        <v>376</v>
-      </c>
-      <c r="E26" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>386</v>
-      </c>
-      <c r="H26" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="J26" s="0" t="s">
-        <v>385</v>
-      </c>
-      <c r="K26" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="M26" s="0" t="s">
+      <c r="C38" s="0" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="N26" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="0" t="s">
-        <v>378</v>
-      </c>
-      <c r="E27" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>389</v>
-      </c>
-      <c r="H27" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="J27" s="0" t="s">
-        <v>388</v>
-      </c>
-      <c r="K27" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="M27" s="0" t="s">
-        <v>391</v>
-      </c>
-      <c r="N27" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="0" t="s">
-        <v>377</v>
-      </c>
-      <c r="E28" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>399</v>
-      </c>
-      <c r="H28" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="J28" s="0" t="s">
-        <v>390</v>
-      </c>
-      <c r="K28" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="M28" s="0" t="s">
-        <v>371</v>
-      </c>
-      <c r="N28" s="1" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G29" s="0" t="s">
-        <v>393</v>
-      </c>
-      <c r="H29" s="1" t="n">
-        <v>20</v>
+      <c r="C39" s="0" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>432</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B25:D25"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Update domains & deities
</commit_message>
<xml_diff>
--- a/city-npc/Ptolus_City_NPC_Encounter.xlsx
+++ b/city-npc/Ptolus_City_NPC_Encounter.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="START" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="607">
   <si>
     <t xml:space="preserve">MORTAL</t>
   </si>
@@ -1818,6 +1818,9 @@
   </si>
   <si>
     <t xml:space="preserve">[generator:deity-28death29-soullink|{}|deity]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[generator:deity-28future29-soullink|{}|deity]</t>
   </si>
   <si>
     <t xml:space="preserve">[generator:deity-28knowledge29-soullink|{}|deity]</t>
@@ -1853,7 +1856,7 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="0%"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1897,6 +1900,16 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
       <family val="0"/>
     </font>
   </fonts>
@@ -1968,7 +1981,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2021,10 +2034,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2034,10 +2043,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2124,9 +2129,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2970000</xdr:colOff>
+      <xdr:colOff>2969640</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>135360</xdr:rowOff>
+      <xdr:rowOff>135000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2136,19 +2141,17 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1033200" y="9322560"/>
-          <a:ext cx="3159720" cy="802440"/>
+          <a:ext cx="3159360" cy="802080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
+            <a:srgbClr val="ffffff"/>
           </a:solidFill>
           <a:round/>
         </a:ln>
@@ -2258,7 +2261,7 @@
       <selection pane="topLeft" activeCell="N7" activeCellId="0" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.6"/>
@@ -2612,7 +2615,7 @@
       <selection pane="topLeft" activeCell="P4" activeCellId="0" sqref="P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.19"/>
@@ -4486,7 +4489,7 @@
       <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
@@ -5303,11 +5306,11 @@
   </sheetPr>
   <dimension ref="A2:AMJ118"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K25" activeCellId="0" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.28"/>
@@ -5497,27 +5500,27 @@
       </c>
       <c r="M4" s="6"/>
       <c r="O4" s="3"/>
-      <c r="P4" s="13" t="n">
+      <c r="P4" s="6" t="n">
         <f aca="false">SUM(P5:P9)</f>
         <v>100</v>
       </c>
-      <c r="S4" s="14" t="n">
+      <c r="S4" s="13" t="n">
         <f aca="false">SUM(S5:S11)</f>
         <v>100</v>
       </c>
-      <c r="V4" s="14" t="n">
+      <c r="V4" s="13" t="n">
         <f aca="false">SUM(V5:V11)</f>
         <v>70</v>
       </c>
-      <c r="Y4" s="14" t="n">
+      <c r="Y4" s="13" t="n">
         <f aca="false">SUM(Y5:Y11)</f>
         <v>100</v>
       </c>
-      <c r="AB4" s="14" t="n">
+      <c r="AB4" s="13" t="n">
         <f aca="false">SUM(AB5:AB11)</f>
         <v>20</v>
       </c>
-      <c r="AE4" s="14" t="n">
+      <c r="AE4" s="13" t="n">
         <f aca="false">SUM(AE5:AE11)</f>
         <v>120</v>
       </c>
@@ -5573,7 +5576,7 @@
       <c r="R5" s="0" t="s">
         <v>358</v>
       </c>
-      <c r="S5" s="14" t="n">
+      <c r="S5" s="13" t="n">
         <v>10</v>
       </c>
       <c r="U5" s="0" t="s">
@@ -5585,7 +5588,7 @@
       <c r="X5" s="0" t="s">
         <v>360</v>
       </c>
-      <c r="Y5" s="14" t="n">
+      <c r="Y5" s="13" t="n">
         <v>10</v>
       </c>
       <c r="AA5" s="0" t="s">
@@ -5711,7 +5714,7 @@
       <c r="R7" s="0" t="s">
         <v>382</v>
       </c>
-      <c r="S7" s="14" t="n">
+      <c r="S7" s="13" t="n">
         <v>10</v>
       </c>
       <c r="U7" s="0" t="s">
@@ -5720,8 +5723,8 @@
       <c r="V7" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="Y7" s="14"/>
-      <c r="AB7" s="14"/>
+      <c r="Y7" s="13"/>
+      <c r="AB7" s="13"/>
       <c r="AD7" s="0" t="s">
         <v>384</v>
       </c>
@@ -5768,7 +5771,7 @@
       <c r="R8" s="0" t="s">
         <v>390</v>
       </c>
-      <c r="S8" s="14" t="n">
+      <c r="S8" s="13" t="n">
         <v>20</v>
       </c>
       <c r="U8" s="0" t="s">
@@ -5777,9 +5780,9 @@
       <c r="V8" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="Y8" s="14"/>
-      <c r="AB8" s="14"/>
-      <c r="AE8" s="14"/>
+      <c r="Y8" s="13"/>
+      <c r="AB8" s="13"/>
+      <c r="AE8" s="13"/>
       <c r="AG8" s="0" t="s">
         <v>392</v>
       </c>
@@ -5816,7 +5819,7 @@
       <c r="R9" s="0" t="s">
         <v>395</v>
       </c>
-      <c r="S9" s="14" t="n">
+      <c r="S9" s="13" t="n">
         <v>10</v>
       </c>
       <c r="U9" s="0" t="s">
@@ -5825,9 +5828,9 @@
       <c r="V9" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="Y9" s="14"/>
-      <c r="AB9" s="14"/>
-      <c r="AE9" s="14"/>
+      <c r="Y9" s="13"/>
+      <c r="AB9" s="13"/>
+      <c r="AE9" s="13"/>
       <c r="AG9" s="0" t="s">
         <v>397</v>
       </c>
@@ -5854,20 +5857,20 @@
         <v>25</v>
       </c>
       <c r="M10" s="11"/>
-      <c r="P10" s="13" t="n">
+      <c r="P10" s="6" t="n">
         <f aca="false">SUM(P11:P15)</f>
         <v>110</v>
       </c>
       <c r="R10" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="S10" s="14" t="n">
-        <v>10</v>
-      </c>
-      <c r="V10" s="14"/>
-      <c r="Y10" s="14"/>
-      <c r="AB10" s="14"/>
-      <c r="AE10" s="14"/>
+      <c r="S10" s="13" t="n">
+        <v>10</v>
+      </c>
+      <c r="V10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="AB10" s="13"/>
+      <c r="AE10" s="13"/>
       <c r="AG10" s="0" t="s">
         <v>400</v>
       </c>
@@ -5888,7 +5891,7 @@
       <c r="P11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="S11" s="14"/>
+      <c r="S11" s="13"/>
       <c r="AG11" s="0" t="s">
         <v>401</v>
       </c>
@@ -5915,7 +5918,7 @@
       <c r="P12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="S12" s="14"/>
+      <c r="S12" s="13"/>
       <c r="AG12" s="0" t="s">
         <v>402</v>
       </c>
@@ -5948,7 +5951,7 @@
       <c r="P13" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="S13" s="14"/>
+      <c r="S13" s="13"/>
       <c r="AG13" s="0" t="s">
         <v>403</v>
       </c>
@@ -5982,7 +5985,7 @@
       <c r="P14" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="S14" s="14"/>
+      <c r="S14" s="13"/>
       <c r="AG14" s="0" t="s">
         <v>405</v>
       </c>
@@ -6003,7 +6006,7 @@
       <c r="P15" s="11" t="n">
         <v>70</v>
       </c>
-      <c r="S15" s="14"/>
+      <c r="S15" s="13"/>
       <c r="AG15" s="0" t="s">
         <v>406</v>
       </c>
@@ -6022,11 +6025,11 @@
         <v>100</v>
       </c>
       <c r="M16" s="11"/>
-      <c r="P16" s="13" t="n">
+      <c r="P16" s="6" t="n">
         <f aca="false">SUM(P17:P21)</f>
         <v>100</v>
       </c>
-      <c r="S16" s="14"/>
+      <c r="S16" s="13"/>
       <c r="AG16" s="0" t="s">
         <v>407</v>
       </c>
@@ -6059,7 +6062,7 @@
       <c r="P17" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="S17" s="14"/>
+      <c r="S17" s="13"/>
       <c r="AG17" s="0" t="s">
         <v>408</v>
       </c>
@@ -6092,7 +6095,7 @@
       <c r="P18" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="S18" s="14"/>
+      <c r="S18" s="13"/>
       <c r="AG18" s="0" t="s">
         <v>410</v>
       </c>
@@ -6113,7 +6116,7 @@
       <c r="P19" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="S19" s="14"/>
+      <c r="S19" s="13"/>
       <c r="AG19" s="0" t="s">
         <v>411</v>
       </c>
@@ -6134,7 +6137,7 @@
       <c r="P20" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="S20" s="14"/>
+      <c r="S20" s="13"/>
       <c r="AG20" s="0" t="s">
         <v>412</v>
       </c>
@@ -6155,7 +6158,7 @@
       <c r="P21" s="11" t="n">
         <v>80</v>
       </c>
-      <c r="S21" s="14"/>
+      <c r="S21" s="13"/>
       <c r="AG21" s="0" t="s">
         <v>413</v>
       </c>
@@ -6165,11 +6168,11 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L22" s="0"/>
-      <c r="P22" s="13" t="n">
+      <c r="P22" s="6" t="n">
         <f aca="false">SUM(P23:P27)</f>
         <v>110</v>
       </c>
-      <c r="S22" s="14"/>
+      <c r="S22" s="13"/>
       <c r="AG22" s="0" t="s">
         <v>414</v>
       </c>
@@ -6188,7 +6191,7 @@
       <c r="P23" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="S23" s="14"/>
+      <c r="S23" s="13"/>
       <c r="AG23" s="0" t="s">
         <v>415</v>
       </c>
@@ -6207,7 +6210,7 @@
       <c r="P24" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="S24" s="14"/>
+      <c r="S24" s="13"/>
       <c r="AG24" s="0" t="s">
         <v>416</v>
       </c>
@@ -6225,7 +6228,7 @@
       <c r="P25" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="S25" s="14"/>
+      <c r="S25" s="13"/>
       <c r="AG25" s="0" t="s">
         <v>417</v>
       </c>
@@ -6243,7 +6246,7 @@
       <c r="P26" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="S26" s="14"/>
+      <c r="S26" s="13"/>
       <c r="AG26" s="0" t="s">
         <v>418</v>
       </c>
@@ -6261,7 +6264,7 @@
       <c r="P27" s="11" t="n">
         <v>90</v>
       </c>
-      <c r="S27" s="14"/>
+      <c r="S27" s="13"/>
       <c r="AG27" s="0" t="s">
         <v>419</v>
       </c>
@@ -6270,7 +6273,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S28" s="14"/>
+      <c r="S28" s="13"/>
       <c r="AG28" s="0" t="s">
         <v>420</v>
       </c>
@@ -6279,7 +6282,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S29" s="14"/>
+      <c r="S29" s="13"/>
       <c r="AG29" s="0" t="s">
         <v>421</v>
       </c>
@@ -6288,7 +6291,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S30" s="14"/>
+      <c r="S30" s="13"/>
       <c r="AG30" s="0" t="s">
         <v>422</v>
       </c>
@@ -6297,7 +6300,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S31" s="14"/>
+      <c r="S31" s="13"/>
       <c r="AG31" s="0" t="s">
         <v>423</v>
       </c>
@@ -6306,7 +6309,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S32" s="14"/>
+      <c r="S32" s="13"/>
       <c r="AG32" s="0" t="s">
         <v>424</v>
       </c>
@@ -6315,7 +6318,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S33" s="14"/>
+      <c r="S33" s="13"/>
       <c r="AG33" s="0" t="s">
         <v>425</v>
       </c>
@@ -6385,7 +6388,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P40" s="0"/>
-      <c r="S40" s="14"/>
+      <c r="S40" s="13"/>
       <c r="AG40" s="0" t="s">
         <v>432</v>
       </c>
@@ -6394,7 +6397,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S41" s="14"/>
+      <c r="S41" s="13"/>
       <c r="AG41" s="0" t="s">
         <v>433</v>
       </c>
@@ -6403,7 +6406,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S42" s="14"/>
+      <c r="S42" s="13"/>
       <c r="AG42" s="0" t="s">
         <v>434</v>
       </c>
@@ -6412,7 +6415,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S43" s="14"/>
+      <c r="S43" s="13"/>
       <c r="AG43" s="0" t="s">
         <v>435</v>
       </c>
@@ -6421,7 +6424,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S44" s="14"/>
+      <c r="S44" s="13"/>
       <c r="AG44" s="0" t="s">
         <v>436</v>
       </c>
@@ -6430,7 +6433,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S45" s="14"/>
+      <c r="S45" s="13"/>
       <c r="AG45" s="0" t="s">
         <v>437</v>
       </c>
@@ -6439,7 +6442,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S46" s="14"/>
+      <c r="S46" s="13"/>
       <c r="AG46" s="0" t="s">
         <v>438</v>
       </c>
@@ -6448,7 +6451,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S47" s="14"/>
+      <c r="S47" s="13"/>
       <c r="AG47" s="0" t="s">
         <v>439</v>
       </c>
@@ -6457,7 +6460,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S48" s="14"/>
+      <c r="S48" s="13"/>
       <c r="AG48" s="0" t="s">
         <v>440</v>
       </c>
@@ -6466,7 +6469,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S49" s="14"/>
+      <c r="S49" s="13"/>
       <c r="AG49" s="0" t="s">
         <v>441</v>
       </c>
@@ -6475,7 +6478,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S50" s="14"/>
+      <c r="S50" s="13"/>
       <c r="AG50" s="0" t="s">
         <v>442</v>
       </c>
@@ -6484,7 +6487,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S51" s="14"/>
+      <c r="S51" s="13"/>
       <c r="AG51" s="0" t="s">
         <v>443</v>
       </c>
@@ -6493,7 +6496,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S52" s="14"/>
+      <c r="S52" s="13"/>
       <c r="AG52" s="0" t="s">
         <v>444</v>
       </c>
@@ -6502,7 +6505,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S53" s="14"/>
+      <c r="S53" s="13"/>
       <c r="AG53" s="0" t="s">
         <v>445</v>
       </c>
@@ -6511,7 +6514,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S54" s="14"/>
+      <c r="S54" s="13"/>
       <c r="AG54" s="0" t="s">
         <v>446</v>
       </c>
@@ -6520,7 +6523,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S55" s="14"/>
+      <c r="S55" s="13"/>
       <c r="AG55" s="0" t="s">
         <v>447</v>
       </c>
@@ -6529,7 +6532,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S56" s="14"/>
+      <c r="S56" s="13"/>
       <c r="AG56" s="0" t="s">
         <v>448</v>
       </c>
@@ -6538,7 +6541,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S57" s="14"/>
+      <c r="S57" s="13"/>
       <c r="AG57" s="0" t="s">
         <v>449</v>
       </c>
@@ -6547,7 +6550,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S58" s="14"/>
+      <c r="S58" s="13"/>
       <c r="AG58" s="0" t="s">
         <v>450</v>
       </c>
@@ -6556,7 +6559,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S59" s="14"/>
+      <c r="S59" s="13"/>
       <c r="AG59" s="0" t="s">
         <v>451</v>
       </c>
@@ -6565,7 +6568,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S60" s="14"/>
+      <c r="S60" s="13"/>
       <c r="AG60" s="0" t="s">
         <v>452</v>
       </c>
@@ -6574,7 +6577,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S61" s="14"/>
+      <c r="S61" s="13"/>
       <c r="AG61" s="0" t="s">
         <v>453</v>
       </c>
@@ -6583,7 +6586,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S62" s="14"/>
+      <c r="S62" s="13"/>
       <c r="AG62" s="0" t="s">
         <v>454</v>
       </c>
@@ -6592,7 +6595,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S63" s="14"/>
+      <c r="S63" s="13"/>
       <c r="AG63" s="0" t="s">
         <v>455</v>
       </c>
@@ -6601,7 +6604,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S64" s="14"/>
+      <c r="S64" s="13"/>
       <c r="AG64" s="0" t="s">
         <v>456</v>
       </c>
@@ -6610,7 +6613,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S65" s="14"/>
+      <c r="S65" s="13"/>
       <c r="AG65" s="0" t="s">
         <v>457</v>
       </c>
@@ -6619,7 +6622,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S66" s="14"/>
+      <c r="S66" s="13"/>
       <c r="AG66" s="0" t="s">
         <v>458</v>
       </c>
@@ -6628,7 +6631,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S67" s="14"/>
+      <c r="S67" s="13"/>
       <c r="AG67" s="0" t="s">
         <v>459</v>
       </c>
@@ -6637,7 +6640,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S68" s="14"/>
+      <c r="S68" s="13"/>
       <c r="AG68" s="0" t="s">
         <v>460</v>
       </c>
@@ -6646,7 +6649,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S69" s="14"/>
+      <c r="S69" s="13"/>
       <c r="AG69" s="0" t="s">
         <v>461</v>
       </c>
@@ -6655,7 +6658,7 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S70" s="14"/>
+      <c r="S70" s="13"/>
       <c r="AG70" s="0" t="s">
         <v>462</v>
       </c>
@@ -6664,7 +6667,7 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S71" s="14"/>
+      <c r="S71" s="13"/>
       <c r="AG71" s="0" t="s">
         <v>463</v>
       </c>
@@ -6673,7 +6676,7 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S72" s="14"/>
+      <c r="S72" s="13"/>
       <c r="AG72" s="0" t="s">
         <v>464</v>
       </c>
@@ -6682,7 +6685,7 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S73" s="14"/>
+      <c r="S73" s="13"/>
       <c r="AG73" s="0" t="s">
         <v>465</v>
       </c>
@@ -6691,7 +6694,7 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S74" s="14"/>
+      <c r="S74" s="13"/>
       <c r="AG74" s="0" t="s">
         <v>466</v>
       </c>
@@ -6700,7 +6703,7 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S75" s="14"/>
+      <c r="S75" s="13"/>
       <c r="AG75" s="0" t="s">
         <v>467</v>
       </c>
@@ -6709,7 +6712,7 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S76" s="14"/>
+      <c r="S76" s="13"/>
       <c r="AG76" s="0" t="s">
         <v>468</v>
       </c>
@@ -6718,7 +6721,7 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S77" s="14"/>
+      <c r="S77" s="13"/>
       <c r="AG77" s="0" t="s">
         <v>469</v>
       </c>
@@ -6727,7 +6730,7 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S78" s="14"/>
+      <c r="S78" s="13"/>
       <c r="AG78" s="0" t="s">
         <v>470</v>
       </c>
@@ -6736,7 +6739,7 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S79" s="14"/>
+      <c r="S79" s="13"/>
       <c r="AG79" s="0" t="s">
         <v>471</v>
       </c>
@@ -6745,7 +6748,7 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S80" s="14"/>
+      <c r="S80" s="13"/>
       <c r="AG80" s="0" t="s">
         <v>472</v>
       </c>
@@ -6754,7 +6757,7 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S81" s="14"/>
+      <c r="S81" s="13"/>
       <c r="AG81" s="0" t="s">
         <v>473</v>
       </c>
@@ -6763,7 +6766,7 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S82" s="14"/>
+      <c r="S82" s="13"/>
       <c r="AG82" s="0" t="s">
         <v>473</v>
       </c>
@@ -6772,7 +6775,7 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S83" s="14"/>
+      <c r="S83" s="13"/>
       <c r="AG83" s="0" t="s">
         <v>474</v>
       </c>
@@ -6781,7 +6784,7 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S84" s="14"/>
+      <c r="S84" s="13"/>
       <c r="AG84" s="0" t="s">
         <v>474</v>
       </c>
@@ -6790,7 +6793,7 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S85" s="14"/>
+      <c r="S85" s="13"/>
       <c r="AG85" s="0" t="s">
         <v>475</v>
       </c>
@@ -6799,7 +6802,7 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S86" s="14"/>
+      <c r="S86" s="13"/>
       <c r="AG86" s="0" t="s">
         <v>475</v>
       </c>
@@ -6808,7 +6811,7 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S87" s="14"/>
+      <c r="S87" s="13"/>
       <c r="AG87" s="0" t="s">
         <v>476</v>
       </c>
@@ -6817,7 +6820,7 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S88" s="14"/>
+      <c r="S88" s="13"/>
       <c r="AG88" s="0" t="s">
         <v>477</v>
       </c>
@@ -6826,7 +6829,7 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S89" s="14"/>
+      <c r="S89" s="13"/>
       <c r="AG89" s="0" t="s">
         <v>478</v>
       </c>
@@ -6835,7 +6838,7 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S90" s="14"/>
+      <c r="S90" s="13"/>
       <c r="AG90" s="0" t="s">
         <v>479</v>
       </c>
@@ -6844,7 +6847,7 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S91" s="14"/>
+      <c r="S91" s="13"/>
       <c r="AG91" s="0" t="s">
         <v>480</v>
       </c>
@@ -6853,7 +6856,7 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S92" s="14"/>
+      <c r="S92" s="13"/>
       <c r="AG92" s="0" t="s">
         <v>481</v>
       </c>
@@ -6862,7 +6865,7 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S93" s="14"/>
+      <c r="S93" s="13"/>
       <c r="AG93" s="0" t="s">
         <v>482</v>
       </c>
@@ -6871,7 +6874,7 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S94" s="14"/>
+      <c r="S94" s="13"/>
       <c r="AG94" s="0" t="s">
         <v>483</v>
       </c>
@@ -6880,7 +6883,7 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S95" s="14"/>
+      <c r="S95" s="13"/>
       <c r="AG95" s="0" t="s">
         <v>484</v>
       </c>
@@ -6889,73 +6892,73 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S96" s="14"/>
+      <c r="S96" s="13"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S97" s="14"/>
+      <c r="S97" s="13"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S98" s="14"/>
+      <c r="S98" s="13"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S99" s="14"/>
+      <c r="S99" s="13"/>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S100" s="14"/>
+      <c r="S100" s="13"/>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S101" s="14"/>
+      <c r="S101" s="13"/>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S102" s="14"/>
+      <c r="S102" s="13"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S103" s="14"/>
+      <c r="S103" s="13"/>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S104" s="14"/>
+      <c r="S104" s="13"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S105" s="14"/>
+      <c r="S105" s="13"/>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S106" s="14"/>
+      <c r="S106" s="13"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S107" s="14"/>
+      <c r="S107" s="13"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S108" s="14"/>
+      <c r="S108" s="13"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S109" s="14"/>
+      <c r="S109" s="13"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S110" s="14"/>
+      <c r="S110" s="13"/>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S111" s="14"/>
+      <c r="S111" s="13"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S112" s="14"/>
+      <c r="S112" s="13"/>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S113" s="14"/>
+      <c r="S113" s="13"/>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S114" s="14"/>
+      <c r="S114" s="13"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S115" s="14"/>
+      <c r="S115" s="13"/>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S116" s="14"/>
+      <c r="S116" s="13"/>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S117" s="14"/>
+      <c r="S117" s="13"/>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S118" s="14"/>
+      <c r="S118" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -6986,11 +6989,11 @@
   </sheetPr>
   <dimension ref="B1:AX56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G35" activeCellId="0" sqref="G35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G36" activeCellId="0" sqref="G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.89"/>
@@ -7017,19 +7020,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="3.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="11.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="2.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="38.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="1.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="38.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="1.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="1.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="27.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="27.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="2.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="28.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="28.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="1.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="38.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="38.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="1.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="29.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="1.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="41.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="41.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="1.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="41.4"/>
   </cols>
@@ -7126,7 +7129,7 @@
       <c r="C3" s="8" t="s">
         <v>502</v>
       </c>
-      <c r="D3" s="13" t="n">
+      <c r="D3" s="6" t="n">
         <f aca="false">SUM(D4:D25)</f>
         <v>349</v>
       </c>
@@ -7187,112 +7190,112 @@
       <c r="D4" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="15" t="n">
+      <c r="E4" s="14" t="n">
         <f aca="false">D4/$D$3</f>
         <v>0.00286532951289398</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>505</v>
       </c>
-      <c r="H4" s="13" t="n">
+      <c r="H4" s="6" t="n">
         <f aca="false">SUM(H5:H34)</f>
         <v>100</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>506</v>
       </c>
-      <c r="K4" s="13" t="n">
+      <c r="K4" s="6" t="n">
         <f aca="false">SUM(K5:K34)</f>
         <v>110</v>
       </c>
       <c r="M4" s="8" t="s">
         <v>507</v>
       </c>
-      <c r="N4" s="13" t="n">
+      <c r="N4" s="6" t="n">
         <f aca="false">SUM(N5:N34)</f>
         <v>100</v>
       </c>
       <c r="P4" s="8" t="s">
         <v>508</v>
       </c>
-      <c r="Q4" s="13" t="n">
+      <c r="Q4" s="6" t="n">
         <f aca="false">SUM(Q5:Q34)</f>
         <v>270</v>
       </c>
       <c r="S4" s="8" t="s">
         <v>490</v>
       </c>
-      <c r="T4" s="13" t="n">
+      <c r="T4" s="6" t="n">
         <f aca="false">SUM(T5:T34)</f>
         <v>180</v>
       </c>
       <c r="V4" s="8" t="s">
         <v>491</v>
       </c>
-      <c r="W4" s="13" t="n">
+      <c r="W4" s="6" t="n">
         <f aca="false">SUM(W5:W34)</f>
         <v>180</v>
       </c>
       <c r="Y4" s="8" t="s">
         <v>492</v>
       </c>
-      <c r="Z4" s="13" t="n">
+      <c r="Z4" s="6" t="n">
         <f aca="false">SUM(Z5:Z34)</f>
         <v>100</v>
       </c>
       <c r="AB4" s="8" t="s">
         <v>493</v>
       </c>
-      <c r="AC4" s="13" t="n">
+      <c r="AC4" s="6" t="n">
         <f aca="false">SUM(AC5:AC34)</f>
         <v>330</v>
       </c>
       <c r="AE4" s="8" t="s">
         <v>494</v>
       </c>
-      <c r="AF4" s="13" t="n">
+      <c r="AF4" s="6" t="n">
         <f aca="false">SUM(AF5:AF34)</f>
         <v>100</v>
       </c>
       <c r="AH4" s="8" t="s">
         <v>495</v>
       </c>
-      <c r="AI4" s="13" t="n">
+      <c r="AI4" s="6" t="n">
         <f aca="false">SUM(AI5:AI34)</f>
         <v>10</v>
       </c>
       <c r="AK4" s="8" t="s">
         <v>496</v>
       </c>
-      <c r="AL4" s="13" t="n">
+      <c r="AL4" s="6" t="n">
         <f aca="false">SUM(AL5:AL34)</f>
         <v>10</v>
       </c>
       <c r="AN4" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="AO4" s="13" t="n">
+      <c r="AO4" s="6" t="n">
         <f aca="false">SUM(AO5:AO34)</f>
         <v>100</v>
       </c>
       <c r="AQ4" s="8" t="s">
         <v>498</v>
       </c>
-      <c r="AR4" s="13" t="n">
+      <c r="AR4" s="6" t="n">
         <f aca="false">SUM(AR5:AR34)</f>
         <v>100</v>
       </c>
       <c r="AT4" s="8" t="s">
         <v>499</v>
       </c>
-      <c r="AU4" s="13" t="n">
+      <c r="AU4" s="6" t="n">
         <f aca="false">SUM(AU5:AU34)</f>
         <v>120</v>
       </c>
       <c r="AW4" s="8" t="s">
         <v>500</v>
       </c>
-      <c r="AX4" s="13" t="n">
+      <c r="AX4" s="6" t="n">
         <f aca="false">SUM(AX5:AX34)</f>
         <v>170</v>
       </c>
@@ -7301,13 +7304,13 @@
       <c r="B5" s="0" t="s">
         <v>509</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>505</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="E5" s="15" t="n">
+      <c r="E5" s="14" t="n">
         <f aca="false">D5/$D$3</f>
         <v>0.0859598853868195</v>
       </c>
@@ -7406,13 +7409,13 @@
       <c r="B6" s="0" t="s">
         <v>521</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>506</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E6" s="15" t="n">
+      <c r="E6" s="14" t="n">
         <f aca="false">D6/$D$3</f>
         <v>0.0573065902578797</v>
       </c>
@@ -7495,13 +7498,13 @@
       <c r="B7" s="0" t="s">
         <v>527</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>507</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E7" s="15" t="n">
+      <c r="E7" s="14" t="n">
         <f aca="false">D7/$D$3</f>
         <v>0.0573065902578797</v>
       </c>
@@ -7581,12 +7584,12 @@
       <c r="D8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E8" s="15" t="n">
+      <c r="E8" s="14" t="n">
         <f aca="false">D8/$D$3</f>
         <v>0.00286532951289398</v>
       </c>
       <c r="G8" s="8"/>
-      <c r="H8" s="13"/>
+      <c r="H8" s="6"/>
       <c r="J8" s="12" t="s">
         <v>539</v>
       </c>
@@ -7594,7 +7597,7 @@
         <v>10</v>
       </c>
       <c r="M8" s="8"/>
-      <c r="N8" s="13"/>
+      <c r="N8" s="6"/>
       <c r="P8" s="12" t="s">
         <v>540</v>
       </c>
@@ -7652,18 +7655,18 @@
       <c r="B9" s="0" t="s">
         <v>546</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>508</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="E9" s="15" t="n">
+      <c r="E9" s="14" t="n">
         <f aca="false">D9/$D$3</f>
         <v>0.0859598853868195</v>
       </c>
       <c r="G9" s="8"/>
-      <c r="H9" s="13"/>
+      <c r="H9" s="6"/>
       <c r="J9" s="12" t="s">
         <v>547</v>
       </c>
@@ -7671,7 +7674,7 @@
         <v>20</v>
       </c>
       <c r="M9" s="8"/>
-      <c r="N9" s="13"/>
+      <c r="N9" s="6"/>
       <c r="P9" s="12" t="s">
         <v>548</v>
       </c>
@@ -7725,18 +7728,18 @@
       <c r="B10" s="0" t="s">
         <v>553</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="15" t="s">
         <v>490</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="E10" s="15" t="n">
+      <c r="E10" s="14" t="n">
         <f aca="false">D10/$D$3</f>
         <v>0.114613180515759</v>
       </c>
       <c r="G10" s="8"/>
-      <c r="H10" s="13"/>
+      <c r="H10" s="6"/>
       <c r="J10" s="12" t="s">
         <v>554</v>
       </c>
@@ -7744,7 +7747,7 @@
         <v>20</v>
       </c>
       <c r="M10" s="8"/>
-      <c r="N10" s="13"/>
+      <c r="N10" s="6"/>
       <c r="P10" s="0" t="s">
         <v>555</v>
       </c>
@@ -7787,18 +7790,18 @@
       <c r="B11" s="0" t="s">
         <v>559</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>491</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="E11" s="15" t="n">
+      <c r="E11" s="14" t="n">
         <f aca="false">D11/$D$3</f>
         <v>0.114613180515759</v>
       </c>
       <c r="G11" s="8"/>
-      <c r="H11" s="13"/>
+      <c r="H11" s="6"/>
       <c r="J11" s="12" t="s">
         <v>560</v>
       </c>
@@ -7806,7 +7809,7 @@
         <v>10</v>
       </c>
       <c r="M11" s="8"/>
-      <c r="N11" s="13"/>
+      <c r="N11" s="6"/>
       <c r="P11" s="12" t="s">
         <v>561</v>
       </c>
@@ -7862,7 +7865,7 @@
       <c r="D12" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="E12" s="15" t="n">
+      <c r="E12" s="14" t="n">
         <f aca="false">D12/$D$3</f>
         <v>0.00286532951289398</v>
       </c>
@@ -7901,13 +7904,13 @@
       <c r="B13" s="0" t="s">
         <v>569</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
         <v>493</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E13" s="15" t="n">
+      <c r="E13" s="14" t="n">
         <f aca="false">D13/$D$3</f>
         <v>0.0573065902578797</v>
       </c>
@@ -7940,7 +7943,7 @@
       <c r="D14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E14" s="15" t="n">
+      <c r="E14" s="14" t="n">
         <f aca="false">D14/$D$3</f>
         <v>0.00286532951289398</v>
       </c>
@@ -7973,7 +7976,7 @@
       <c r="D15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E15" s="15" t="n">
+      <c r="E15" s="14" t="n">
         <f aca="false">D15/$D$3</f>
         <v>0.00286532951289398</v>
       </c>
@@ -8006,7 +8009,7 @@
       <c r="D16" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E16" s="15" t="n">
+      <c r="E16" s="14" t="n">
         <f aca="false">D16/$D$3</f>
         <v>0.00286532951289398</v>
       </c>
@@ -8039,7 +8042,7 @@
       <c r="D17" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E17" s="15" t="n">
+      <c r="E17" s="14" t="n">
         <f aca="false">D17/$D$3</f>
         <v>0.00286532951289398</v>
       </c>
@@ -8060,13 +8063,13 @@
       <c r="B18" s="0" t="s">
         <v>583</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="15" t="s">
         <v>495</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E18" s="15" t="n">
+      <c r="E18" s="14" t="n">
         <f aca="false">D18/$D$3</f>
         <v>0.0573065902578797</v>
       </c>
@@ -8081,13 +8084,13 @@
       <c r="B19" s="0" t="s">
         <v>584</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="15" t="s">
         <v>496</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E19" s="15" t="n">
+      <c r="E19" s="14" t="n">
         <f aca="false">D19/$D$3</f>
         <v>0.0573065902578797</v>
       </c>
@@ -8102,13 +8105,13 @@
       <c r="B20" s="0" t="s">
         <v>586</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="15" t="s">
         <v>497</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="E20" s="15" t="n">
+      <c r="E20" s="14" t="n">
         <f aca="false">D20/$D$3</f>
         <v>0.0859598853868195</v>
       </c>
@@ -8118,13 +8121,13 @@
       <c r="B21" s="0" t="s">
         <v>587</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="15" t="s">
         <v>498</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E21" s="15" t="n">
+      <c r="E21" s="14" t="n">
         <f aca="false">D21/$D$3</f>
         <v>0.0573065902578797</v>
       </c>
@@ -8140,7 +8143,7 @@
       <c r="D22" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E22" s="15" t="n">
+      <c r="E22" s="14" t="n">
         <f aca="false">D22/$D$3</f>
         <v>0.00286532951289398</v>
       </c>
@@ -8150,13 +8153,13 @@
       <c r="B23" s="0" t="s">
         <v>590</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="15" t="s">
         <v>499</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E23" s="15" t="n">
+      <c r="E23" s="14" t="n">
         <f aca="false">D23/$D$3</f>
         <v>0.0573065902578797</v>
       </c>
@@ -8172,7 +8175,7 @@
       <c r="D24" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E24" s="15" t="n">
+      <c r="E24" s="14" t="n">
         <f aca="false">D24/$D$3</f>
         <v>0.00286532951289398</v>
       </c>
@@ -8182,13 +8185,13 @@
       <c r="B25" s="0" t="s">
         <v>593</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="15" t="s">
         <v>500</v>
       </c>
       <c r="D25" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="E25" s="15" t="n">
+      <c r="E25" s="14" t="n">
         <f aca="false">D25/$D$3</f>
         <v>0.0859598853868195</v>
       </c>
@@ -8215,7 +8218,7 @@
       <c r="C29" s="8" t="s">
         <v>502</v>
       </c>
-      <c r="D29" s="13"/>
+      <c r="D29" s="6"/>
       <c r="T29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8229,7 +8232,7 @@
       <c r="T30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="15" t="s">
         <v>509</v>
       </c>
       <c r="C31" s="0" t="s">
@@ -8238,7 +8241,7 @@
       <c r="T31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="15" t="s">
         <v>521</v>
       </c>
       <c r="C32" s="0" t="s">
@@ -8247,11 +8250,11 @@
       <c r="T32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>507</v>
+        <v>598</v>
       </c>
       <c r="T33" s="1"/>
     </row>
@@ -8265,29 +8268,29 @@
       <c r="T34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="15" t="s">
         <v>546</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="T35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="15" t="s">
         <v>553</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="T36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="15" t="s">
         <v>559</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="T37" s="1"/>
     </row>
@@ -8302,11 +8305,11 @@
       <c r="T38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="15" t="s">
         <v>569</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="T39" s="1"/>
     </row>
@@ -8347,38 +8350,38 @@
       <c r="T43" s="1"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="15" t="s">
         <v>583</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>495</v>
+        <v>516</v>
       </c>
       <c r="T44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="15" t="s">
         <v>584</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>496</v>
+        <v>517</v>
       </c>
       <c r="T45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="15" t="s">
         <v>586</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="T46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="15" t="s">
         <v>587</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="T47" s="1"/>
     </row>
@@ -8392,16 +8395,16 @@
       <c r="T48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="16" t="s">
+      <c r="B49" s="15" t="s">
         <v>590</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="T49" s="1"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="12" t="s">
         <v>591</v>
       </c>
       <c r="C50" s="0" t="s">
@@ -8410,11 +8413,11 @@
       <c r="T50" s="1"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="16" t="s">
+      <c r="B51" s="15" t="s">
         <v>593</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="T51" s="1"/>
     </row>

</xml_diff>

<commit_message>
add origin csv files
</commit_message>
<xml_diff>
--- a/city-npc/Ptolus_City_NPC_Encounter.xlsx
+++ b/city-npc/Ptolus_City_NPC_Encounter.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="START" sheetId="1" state="visible" r:id="rId2"/>
@@ -2542,7 +2542,7 @@
   <dimension ref="A2:AMJ25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H22" activeCellId="1" sqref="H5 H22"/>
+      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2896,8 +2896,8 @@
   </sheetPr>
   <dimension ref="B1:AE121"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="1" sqref="H5 F26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5432,7 +5432,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="1" sqref="H5 E23"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5686,8 +5686,8 @@
   </sheetPr>
   <dimension ref="A2:AMJ118"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="1" sqref="H5 H17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7370,7 +7370,7 @@
   <dimension ref="A1:AY56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G25" activeCellId="1" sqref="H5 G25"/>
+      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11090,7 +11090,7 @@
   <dimension ref="A1:Q114"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J34" activeCellId="1" sqref="H5 J34"/>
+      <selection pane="topLeft" activeCell="J34" activeCellId="0" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12088,7 +12088,7 @@
   <dimension ref="A1:W131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M8" activeCellId="1" sqref="H5 M8"/>
+      <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>